<commit_message>
Added Pipeline for Merged Data
</commit_message>
<xml_diff>
--- a/Data/Sorted_Inactivation/sortingNotes/SortingNotes_20190516_B.xlsx
+++ b/Data/Sorted_Inactivation/sortingNotes/SortingNotes_20190516_B.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LaboDancauseDS\home\sortedDataMatlabFormat\MonkeyB\Note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14252\NHP Data Analysis\Data\Sorted_Inactivation\sortingNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647EE07D-658B-43BE-90A3-1F2ED601FB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K227" sqref="K227"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="D200" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="D193" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
@@ -5056,10 +5057,7 @@
         <v>65</v>
       </c>
       <c r="C194">
-        <v>1</v>
-      </c>
-      <c r="D194">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I194" s="2">
         <v>2</v>

</xml_diff>